<commit_message>
[FIX] FIX test init db groovy
</commit_message>
<xml_diff>
--- a/src/test/resources/script.db/2018-5-3-devops.xlsx
+++ b/src/test/resources/script.db/2018-5-3-devops.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t xml:space="preserve">devops_app_template</t>
   </si>
@@ -98,6 +98,9 @@
     <t xml:space="preserve">devops_user</t>
   </si>
   <si>
+    <t xml:space="preserve">#iam_user_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">gitlab_user_id</t>
   </si>
 </sst>
@@ -259,9 +262,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.0042918454936"/>
-    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="18.1673819742489"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="23.5064377682403"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.9785407725322"/>
+    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="19.3047210300429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="25.0944206008584"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -287,14 +290,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="18.1673819742489"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="104.017167381974"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="171.467811158798"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="117.643776824034"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="112.875536480687"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="96.9742489270386"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="123.321888412017"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="18.1673819742489"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="19.3047210300429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="111.171673819742"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="183.390557939914"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="125.81974248927"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="120.708154506438"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="103.789699570815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="131.952789699571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="19.3047210300429"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,16 +406,16 @@
   <dimension ref="D7:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.0128755364807"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.3218884120172"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0128755364807"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="142.510729613734"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0128755364807"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6952789699571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="93.343347639485"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6952789699571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="152.50643776824"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6952789699571"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,10 +423,10 @@
         <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>